<commit_message>
Performed some speed optimizations to speed up the calculation of feature vectors, in particular skipping the slow trim_outliers method.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="carNight1 (1)" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="carNight1 (2)" sheetId="4" r:id="rId4"/>
     <sheet name="carNight2 (2)" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -11133,6 +11134,1596 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>carNight2.wav</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> w</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ith Null Data (Wind,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Computer Noise)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$A$1:$A$437</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="437"/>
+                <c:pt idx="0">
+                  <c:v>-2.2233360002280201E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.7947830845141098E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.2280736823115698E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.4969996825023802E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.0870477572171699E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.63707702630533E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.16738331328727E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.35165211932102E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9417292828463101E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5107174271416399E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.37651396515632E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.98370838884891E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-3.2111370031284697E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.90582658894281E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-3.4186776907303297E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-3.0804853234057499E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1346644638140103E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.6839900693293998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-6.2791717691716899E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-4.8663608529630302E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.8724959128204796E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.50177228997216E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5.5674633262752602E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-2.5400589208853901E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.0713846703515301E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.4351400333167401E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-2.6910144282572501E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.28726970725337E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.10276680407864E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-5.2482794114348599E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-2.6894136795085E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.4990760788750701E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-6.37108395914927E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.38661324584932499</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.26660738003522799</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-2.6473734907367302E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.5385934698579698E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.4304815432633801E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.66477294469055E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-8.3487341179867194E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.9552047132312E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.30277599499438101</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-2.1406020426822599E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.6948194150895102E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-3.1354404281472598E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-2.92451960190101E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-3.2211274537796097E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-3.02464799589049E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-3.1531685396065198E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-3.4538771900750401E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-4.9670135032923203E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-7.3540652386696007E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-3.1741767108429603E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-1.9021906780109302E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-1.8889582807524799E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-4.2280193458429399E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.49875920961399E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.155098725671096</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.3795205817146299E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.138703350044104</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.68178418939244E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.7773589237552999E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.1246649212052701E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.2548889452360301E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-3.0345233189327898E-3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-0.14282575209406001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-1.49382877813992E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-2.4328372499654499E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-9.6098665738127108E-3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-2.5013992131563901E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-1.8754348770590699E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.0288281895391402E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.40781993061476E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-2.5862210310910301E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.16551548700803501</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-1.50819017214093E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-2.3894337840076298E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.152313231900087</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.28013435252922703</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9.3760480156216998E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-1.8466644987749199E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-1.72958040951459E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-2.41419263154448E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-1.5692094265373002E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.117432553581254</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-2.4437366889789699E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.116352850002099</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-1.10753095553511E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-5.1720200310272002E-3</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-2.2254133262662901E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-2.7916386992027701E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-8.8996037689679404E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-2.2930435752455802E-3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-1.6805313796336301E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.4988816323167198E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-2.3569114417936399E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-1.6386486199169801E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.7228659116041E-3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-3.520216984071E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-1.7457268588303699E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-3.1407007139137799E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.9109391721571599E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5.33152738662149E-3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2.6667492140791602E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.6303441816845499E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>8.9586428952985095E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9.4661733298554793E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-6.5180609957126599E-3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.33236086598499E-3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-1.0456980782923101E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-2.1367353667836798E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-9.4199268579357801E-3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-1.94679496159973E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-3.3795452269721098E-3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>8.7400443596428509E-3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2.5418439540735201E-2</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.8663861223903799E-2</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-1.4488025313100301E-2</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7.5255639988877103E-3</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>-8.0936120016117802E-3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.3212216170567699E-2</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5.96244531679867E-3</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2.2405755469817001E-2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2.44782898336687E-2</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>4.3362910026630001E-2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.60926143531446E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3.02959580717925E-2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3.3595943754671301E-2</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>3.4647301105455899E-2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>4.1177564236584099E-2</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.07516829000516E-2</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2.73769230553573E-2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4.13801530117726E-2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>5.1864179819563101E-2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.6052989196257802E-2</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.6214435092700598E-2</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.7644766674973701E-2</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>7.6607969170693402E-2</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>5.7365615991197702E-2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>5.7937105728886197E-2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.0032970361876299E-2</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>8.4477132965773E-2</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4.2156991282445697E-2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>3.4372043151753899E-2</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.8902792184377798E-2</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>5.0723609289184901E-2</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2.8408991706681999E-2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>5.4827646619030499E-3</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.0714598718417299E-2</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3.8333008073360798E-2</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>6.1325362137947703E-2</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>8.2572355139719604E-3</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>7.8088874445205902E-2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>6.0098576303478903E-2</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3.2073211731798203E-2</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>6.1000432409259099E-2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2.6051418066704E-2</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>5.0393095841840499E-2</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.102446118318295</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>5.0286484945433599E-2</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>6.9853566225074895E-2</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>8.2780761545109494E-2</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>9.1605675200250605E-2</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.14282446843027199</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.189563202791527</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.149521336982194</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.25996136129653802</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.182696398069921</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.20610967473717701</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.16481325594747101</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.26444663456121398</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.237880464834137</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.19287958489763199</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.47018549400097398</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.31564101694431601</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.32971578990760902</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.25497161753686598</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.37809539858591301</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.372419310350729</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.38510324194088502</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.45331958994197502</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.56176659665412298</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.62847939201290104</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.516380987449919</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.52848453125154604</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.69288409416860297</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.735373853069762</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.79629015908134504</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.73539192887510596</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.63051329786422206</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.74692077311701699</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.76822564380806901</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.781352735778027</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.70997657084311505</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.76528545596690301</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.74687189350175898</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.78956254825844796</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.72113290743568603</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.83258835626869199</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.888710491460736</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.73966774910194</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.80229542352141903</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.67933446798128605</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.618391621515193</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.77641694863607102</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.53088424507532195</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.57729712356266805</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.54132061305075696</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.755964590380648</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.64284455102493998</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.58512414575358895</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.74634342575503398</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.62624090975325297</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.741161211405437</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.458401963368258</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.61521127395283604</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.65817180000397102</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.64473749388341095</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.78813551854179198</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.612191239195641</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.65253540353033901</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.50656576564556099</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.68729329735899303</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.65459615972357599</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.80717886513071602</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.60132215929648003</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.60253394045976005</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.77028924475333804</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.74151199309729798</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.72276828890174005</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.90045092062519905</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.73455350860886204</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.85534775923831097</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.75346294452345497</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.81051174863923503</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.87739498379487202</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.75178119580244795</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.83913472617195395</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.77656340809010704</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.71227868944349304</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.64508193423346805</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.8995895069773</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2.00913958099677</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>2.85505516717916</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1.3888539984582799</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.37232136129128601</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>-2.87613234393196E-2</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.55305137532397497</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.61665571838739897</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.54856232363148205</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>-3.14304953364258E-2</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>-2.48380665105477E-2</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2.38427967989738E-2</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>7.2573764142137703E-2</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>5.3790071704356401E-2</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>-4.6455056602519501E-2</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>-4.4422668843682997E-2</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>-3.7930223515504999E-2</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>-3.6455507558659297E-2</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>-3.77370434018044E-2</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>-3.6299401239209501E-2</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>-2.4038473792049701E-2</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>-2.46159861738241E-2</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>-4.1802792679843499E-2</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>-3.7887417508037403E-2</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>-9.4487905724029597E-2</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>-3.6540537749635602E-2</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1.51666371578117E-2</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>-2.21652868167211E-2</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>-2.44914422372986E-2</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>-3.5652020680012102E-2</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>-3.7664627342836397E-2</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>-4.2002045884173299E-2</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>-3.9080349031578601E-2</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>-3.9589753084131103E-2</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>-3.97300760223053E-2</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>7.6285418305953104E-2</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>-2.72610397821423E-2</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>-3.9285725170691801E-2</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>-3.4025991868071002E-2</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>-4.8119939294106601E-2</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>-2.9798702809135099E-2</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>-7.1529630471170003E-2</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>-5.8606410236002299E-2</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>-5.6246464324577701E-2</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>0.59669853789740801</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>-4.4577346887053303E-2</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>-6.9560773801190495E-2</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>-2.8366283008842499E-2</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>-3.9652514656050901E-2</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>-0.149512081313876</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>-0.24104335349735601</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>-4.7603478679616097E-2</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>-7.8180916790083196E-2</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>-3.4439749478278901E-2</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>-5.1052608761017401E-2</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>-3.0171706046762201E-2</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>0.11906864888671601</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>-3.09049013853646E-2</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>6.9328483666280097E-2</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>0.196038243985483</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>-3.5802969777265603E-2</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>-1.9656906719795801E-2</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>-0.214300605655456</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>-2.0176855355832898E-2</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>-3.78075352686306E-2</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>-0.152550280257856</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>-4.5418218986188301E-2</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>-0.14573333288600099</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>3.48499120979864E-2</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>-0.16025664916103599</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>-0.20266784003161101</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>-0.27673571291007398</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>-6.6764456292139299E-2</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>-0.18146630524520899</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>-0.14324812269673501</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>7.74342246820479E-2</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>-0.177616562190369</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>-0.15194748504686501</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>-0.140596363474494</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>-0.17299551317384901</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>-0.16445780881154401</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>-0.14341622534097101</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>-0.188829269617105</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>-0.139181483191231</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>-0.16679780054944099</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>0.15435014240430101</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>-0.163480755307995</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>-1.90783004338578E-2</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>-2.15485719062102E-2</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>3.7358628541623601E-3</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>0.102554485725075</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>0.104965478849164</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>0.14079981988384399</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>9.6869548442124601E-2</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>8.9455305451589306E-2</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>2.34342632292113E-2</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>4.1586341303164201E-2</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>-3.34940871712502E-2</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>-3.5889157778851301E-2</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>-2.75299677653629E-2</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>0.43677686050708497</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>8.0978890688460595E-3</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>-3.39313866232758E-2</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>-2.8619909799285501E-2</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>-2.47387280065645E-2</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>-3.5324413379345901E-2</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>-1.40085827389285E-2</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>-3.2919319676108803E-2</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>-5.0729106496471402E-2</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>-2.8151126371740401E-2</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>-3.7172933140239901E-2</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>-1.0531532545346599E-2</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>-3.5498157971021897E-2</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>-1.7585090771988401E-2</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>-3.2444836923056601E-2</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>-2.0589106246270202E-2</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>-3.4675029883853299E-2</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>-2.3486036909217699E-2</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>-3.9067599747430397E-2</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>-2.5187881674115099E-2</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>-6.6253937210218494E-2</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>-5.0745255262896902E-2</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>-3.5975825974482803E-2</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>-9.5492730743397897E-2</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>-6.2450479287123897E-2</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>-4.5211937861602602E-2</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>-4.82983157671154E-2</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>-9.4714810016932993E-2</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>-6.4014175303567497E-2</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>-6.2575605129309098E-2</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>-6.9887994825496E-2</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>-5.9403136640823702E-2</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>-3.04382477973612E-2</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>-3.67396752734378E-2</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>-4.3527196268489103E-2</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>-3.6261681081700303E-2</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>-4.1187770549480897E-2</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>-6.3983097572134504E-3</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>-0.17656859444667899</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>-0.16893553427792601</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>-4.5669194061205801E-2</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>-2.4564994085332598E-2</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>-9.6256680403551502E-3</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>0.21711219061221501</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>-2.6692620990637801E-2</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>-0.16667688572786701</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>-0.159813798861488</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>-0.15021140396014199</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>-0.174485361387894</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>6.0189890214003401E-2</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>-0.135948396539258</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>-0.132565569351829</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>-0.159900626615362</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>-0.141853174451822</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>-5.7134327662862201E-2</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>-3.1472922139014203E-2</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>-1.69207565796968E-2</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>-1.8574811398523398E-2</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>-3.2950784938844499E-2</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>-2.0732579504758201E-2</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>-2.50623330218155E-2</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>-5.8578405388619498E-2</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>-5.0071842456987301E-3</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>-0.18216793473786699</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>-0.12753979271527399</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>-3.0043058388798598E-2</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>-0.171060458810331</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>-0.174256944504601</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>-0.16735620500878401</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>-0.17387786076696499</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>-5.2869643919027801E-3</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>-9.3971997882565106E-2</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>-0.14867764021857099</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>-0.15748040488200199</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>-0.15802587876975499</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>-1.38700468082816E-2</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>-5.0810267338753101E-2</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>-2.30223720690024E-2</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>-1.0471168485863399E-2</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>-1.6778491280157001E-2</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>-4.4485491000372503E-2</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>-2.1871454013059601E-2</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>-9.6625477276647304E-2</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>9.8972316473955699E-2</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>3.2405621823320498E-2</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>-4.7274372158971701E-3</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>-9.8599465455755601E-3</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>-6.1577502612660699E-2</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>-3.6019306412708299E-2</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>-9.1563401790469998E-2</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>-5.6289960126802603E-2</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>-4.4134851894444001E-2</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>-3.1285332444206899E-2</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>-3.2244275772148702E-2</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>-3.12909076853711E-2</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>-1.7337633029103201E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="312414448"/>
+        <c:axId val="312417248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="312414448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312417248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="312417248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312414448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11334,6 +12925,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -14469,6 +16100,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -14662,6 +16809,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>538161</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -26329,7 +28511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -29847,4 +32029,2205 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A437"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-2.2233360002280201E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-3.7947830845141098E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-3.2280736823115698E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-3.4969996825023802E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-3.0870477572171699E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-2.63707702630533E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-1.16738331328727E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-1.35165211932102E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.9417292828463101E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2.5107174271416399E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7.37651396515632E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-1.98370838884891E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-3.2111370031284697E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-2.90582658894281E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-3.4186776907303297E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-3.0804853234057499E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.1346644638140103E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-2.6839900693293998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-6.2791717691716899E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-4.8663608529630302E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6.8724959128204796E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-1.50177228997216E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-5.5674633262752602E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-2.5400589208853901E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-3.0713846703515301E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-3.4351400333167401E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-2.6910144282572501E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-1.28726970725337E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-3.10276680407864E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>-5.2482794114348599E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>-2.6894136795085E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>-2.4990760788750701E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-6.37108395914927E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.38661324584932499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.26660738003522799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-2.6473734907367302E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3.5385934698579698E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>-1.4304815432633801E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5.66477294469055E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>-8.3487341179867194E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>-2.9552047132312E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.30277599499438101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>-2.1406020426822599E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-1.6948194150895102E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-3.1354404281472598E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>-2.92451960190101E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>-3.2211274537796097E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>-3.02464799589049E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>-3.1531685396065198E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>-3.4538771900750401E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>-4.9670135032923203E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>-7.3540652386696007E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>-3.1741767108429603E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>-1.9021906780109302E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>-1.8889582807524799E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>-4.2280193458429399E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3.49875920961399E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>-0.155098725671096</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>4.3795205817146299E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>-0.138703350044104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1.68178418939244E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2.7773589237552999E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2.1246649212052701E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1.2548889452360301E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>-3.0345233189327898E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>-0.14282575209406001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>-1.49382877813992E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>-2.4328372499654499E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>-9.6098665738127108E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>-2.5013992131563901E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>-1.8754348770590699E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2.0288281895391402E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2.40781993061476E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>-2.5862210310910301E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>-0.16551548700803501</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>-1.50819017214093E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>-2.3894337840076298E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>-0.152313231900087</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0.28013435252922703</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>9.3760480156216998E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>-1.8466644987749199E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>-1.72958040951459E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>-2.41419263154448E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>-1.5692094265373002E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>-0.117432553581254</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>-2.4437366889789699E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>-0.116352850002099</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>-1.10753095553511E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>-5.1720200310272002E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>-2.2254133262662901E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>-2.7916386992027701E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>-8.8996037689679404E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>-2.2930435752455802E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>-1.6805313796336301E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2.4988816323167198E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>-2.3569114417936399E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>-1.6386486199169801E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2.7228659116041E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>-3.520216984071E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>-1.7457268588303699E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>-3.1407007139137799E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2.9109391721571599E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>5.33152738662149E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2.6667492140791602E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1.6303441816845499E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>8.9586428952985095E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>9.4661733298554793E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>-6.5180609957126599E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1.33236086598499E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>-1.0456980782923101E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>-2.1367353667836798E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>-9.4199268579357801E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>-1.94679496159973E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>-3.3795452269721098E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>8.7400443596428509E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2.5418439540735201E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>3.8663861223903799E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>-1.4488025313100301E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>7.5255639988877103E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>-8.0936120016117802E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1.3212216170567699E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>5.96244531679867E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2.2405755469817001E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2.44782898336687E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>4.3362910026630001E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>2.60926143531446E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>3.02959580717925E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>3.3595943754671301E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>3.4647301105455899E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>4.1177564236584099E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>2.07516829000516E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>2.73769230553573E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>4.13801530117726E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>5.1864179819563101E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>3.6052989196257802E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2.6214435092700598E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1.7644766674973701E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>7.6607969170693402E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>5.7365615991197702E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>5.7937105728886197E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>3.0032970361876299E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>8.4477132965773E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>4.2156991282445697E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>3.4372043151753899E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>4.8902792184377798E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>5.0723609289184901E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>2.8408991706681999E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>5.4827646619030499E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>2.0714598718417299E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>3.8333008073360798E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>6.1325362137947703E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>8.2572355139719604E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>7.8088874445205902E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>6.0098576303478903E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>3.2073211731798203E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>6.1000432409259099E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>2.6051418066704E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>5.0393095841840499E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>0.102446118318295</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>5.0286484945433599E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>6.9853566225074895E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>8.2780761545109494E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>9.1605675200250605E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>0.14282446843027199</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>0.189563202791527</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>0.149521336982194</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>0.25996136129653802</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>0.182696398069921</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>0.20610967473717701</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>0.16481325594747101</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>0.26444663456121398</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>0.237880464834137</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>0.19287958489763199</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>0.47018549400097398</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>0.31564101694431601</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>0.32971578990760902</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>0.25497161753686598</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>0.37809539858591301</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>0.372419310350729</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>0.38510324194088502</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>0.45331958994197502</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>0.56176659665412298</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>0.62847939201290104</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>0.516380987449919</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>0.52848453125154604</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>0.69288409416860297</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>0.735373853069762</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>0.79629015908134504</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>0.73539192887510596</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>0.63051329786422206</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>0.74692077311701699</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>0.76822564380806901</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>0.781352735778027</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>0.70997657084311505</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>0.76528545596690301</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>0.74687189350175898</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>0.78956254825844796</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>0.72113290743568603</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>0.83258835626869199</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>0.888710491460736</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>0.73966774910194</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>0.80229542352141903</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>0.67933446798128605</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>0.618391621515193</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>0.77641694863607102</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>0.53088424507532195</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>0.57729712356266805</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>0.54132061305075696</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>0.755964590380648</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>0.64284455102493998</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>0.58512414575358895</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>0.74634342575503398</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>0.62624090975325297</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>0.741161211405437</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>0.458401963368258</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>0.61521127395283604</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>0.65817180000397102</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>0.64473749388341095</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>0.78813551854179198</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>0.612191239195641</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>0.65253540353033901</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>0.50656576564556099</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>0.68729329735899303</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>0.65459615972357599</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>0.80717886513071602</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>0.60132215929648003</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>0.60253394045976005</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>0.77028924475333804</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>0.74151199309729798</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>0.72276828890174005</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>0.90045092062519905</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>0.73455350860886204</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>0.85534775923831097</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>0.75346294452345497</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>0.81051174863923503</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>0.87739498379487202</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>0.75178119580244795</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>0.83913472617195395</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>0.77656340809010704</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>0.71227868944349304</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>0.64508193423346805</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>0.8995895069773</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>2.00913958099677</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>2.85505516717916</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>1.3888539984582799</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>0.37232136129128601</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>-2.87613234393196E-2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>0.55305137532397497</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>0.61665571838739897</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>0.54856232363148205</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>-3.14304953364258E-2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>-2.48380665105477E-2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>2.38427967989738E-2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>7.2573764142137703E-2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>5.3790071704356401E-2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>-4.6455056602519501E-2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>-4.4422668843682997E-2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>-3.7930223515504999E-2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>-3.6455507558659297E-2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>-3.77370434018044E-2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>-3.6299401239209501E-2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>-2.4038473792049701E-2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>-2.46159861738241E-2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>-4.1802792679843499E-2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>-3.7887417508037403E-2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>-9.4487905724029597E-2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>-3.6540537749635602E-2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>1.51666371578117E-2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>-2.21652868167211E-2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>-2.44914422372986E-2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>-3.5652020680012102E-2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>-3.7664627342836397E-2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>-4.2002045884173299E-2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>-3.9080349031578601E-2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>-3.9589753084131103E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>-3.97300760223053E-2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>7.6285418305953104E-2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>-2.72610397821423E-2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>-3.9285725170691801E-2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>-3.4025991868071002E-2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>-4.8119939294106601E-2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>-2.9798702809135099E-2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>-7.1529630471170003E-2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>-5.8606410236002299E-2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>-5.6246464324577701E-2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>0.59669853789740801</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>-4.4577346887053303E-2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>-6.9560773801190495E-2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>-2.8366283008842499E-2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>-3.9652514656050901E-2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>-0.149512081313876</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>-0.24104335349735601</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>-4.7603478679616097E-2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>-7.8180916790083196E-2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>-3.4439749478278901E-2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>-5.1052608761017401E-2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>-3.0171706046762201E-2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>0.11906864888671601</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>-3.09049013853646E-2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>6.9328483666280097E-2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>0.196038243985483</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>-3.5802969777265603E-2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>-1.9656906719795801E-2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>-0.214300605655456</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>-2.0176855355832898E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>-3.78075352686306E-2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>-0.152550280257856</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>-4.5418218986188301E-2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>-0.14573333288600099</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>3.48499120979864E-2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>-0.16025664916103599</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>-0.20266784003161101</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>-0.27673571291007398</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>-6.6764456292139299E-2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>-0.18146630524520899</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>-0.14324812269673501</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>7.74342246820479E-2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>-0.177616562190369</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>-0.15194748504686501</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>-0.140596363474494</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>-0.17299551317384901</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>-0.16445780881154401</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>-0.14341622534097101</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>-0.188829269617105</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>-0.139181483191231</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>-0.16679780054944099</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>0.15435014240430101</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>-0.163480755307995</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>-1.90783004338578E-2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>-2.15485719062102E-2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>3.7358628541623601E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>0.102554485725075</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>0.104965478849164</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>0.14079981988384399</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>9.6869548442124601E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>8.9455305451589306E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>2.34342632292113E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>4.1586341303164201E-2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>-3.34940871712502E-2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>-3.5889157778851301E-2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>-2.75299677653629E-2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>0.43677686050708497</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>8.0978890688460595E-3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>-3.39313866232758E-2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>-2.8619909799285501E-2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>-2.47387280065645E-2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>-3.5324413379345901E-2</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>-1.40085827389285E-2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>-3.2919319676108803E-2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>-5.0729106496471402E-2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>-2.8151126371740401E-2</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>-3.7172933140239901E-2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>-1.0531532545346599E-2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>-3.5498157971021897E-2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>-1.7585090771988401E-2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>-3.2444836923056601E-2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>-2.0589106246270202E-2</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>-3.4675029883853299E-2</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>-2.3486036909217699E-2</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>-3.9067599747430397E-2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>-2.5187881674115099E-2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>-6.6253937210218494E-2</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>-5.0745255262896902E-2</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>-3.5975825974482803E-2</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>-9.5492730743397897E-2</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>-6.2450479287123897E-2</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>-4.5211937861602602E-2</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>-4.82983157671154E-2</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>-9.4714810016932993E-2</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>-6.4014175303567497E-2</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>-6.2575605129309098E-2</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>-6.9887994825496E-2</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>-5.9403136640823702E-2</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>-3.04382477973612E-2</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>-3.67396752734378E-2</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>-4.3527196268489103E-2</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>-3.6261681081700303E-2</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>-4.1187770549480897E-2</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>-6.3983097572134504E-3</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>-0.17656859444667899</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>-0.16893553427792601</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>-4.5669194061205801E-2</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>-2.4564994085332598E-2</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>-9.6256680403551502E-3</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>0.21711219061221501</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>-2.6692620990637801E-2</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>-0.16667688572786701</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>-0.159813798861488</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>-0.15021140396014199</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>-0.174485361387894</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>6.0189890214003401E-2</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>-0.135948396539258</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>-0.132565569351829</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>-0.159900626615362</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>-0.141853174451822</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>-5.7134327662862201E-2</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>-3.1472922139014203E-2</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>-1.69207565796968E-2</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>-1.8574811398523398E-2</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>-3.2950784938844499E-2</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>-2.0732579504758201E-2</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>-2.50623330218155E-2</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>-5.8578405388619498E-2</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>-5.0071842456987301E-3</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>-0.18216793473786699</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>-0.12753979271527399</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>-3.0043058388798598E-2</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>-0.171060458810331</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>-0.174256944504601</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>-0.16735620500878401</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>-0.17387786076696499</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>-5.2869643919027801E-3</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>-9.3971997882565106E-2</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>-0.14867764021857099</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>-0.15748040488200199</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>-0.15802587876975499</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>-1.38700468082816E-2</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>-5.0810267338753101E-2</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>-2.30223720690024E-2</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>-1.0471168485863399E-2</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>-1.6778491280157001E-2</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>-4.4485491000372503E-2</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>-2.1871454013059601E-2</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>-9.6625477276647304E-2</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>9.8972316473955699E-2</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>3.2405621823320498E-2</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>-4.7274372158971701E-3</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>-9.8599465455755601E-3</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>-6.1577502612660699E-2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>-3.6019306412708299E-2</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>-9.1563401790469998E-2</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>-5.6289960126802603E-2</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>-4.4134851894444001E-2</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>-3.1285332444206899E-2</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>-3.2244275772148702E-2</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>-3.12909076853711E-2</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>-1.7337633029103201E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified normalization methods, fixed graphical display of analysis results, and switched to more efficient XML-based classifier storage method.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="carNight1 (1)" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="carNight2 (2)" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="9" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -12724,6 +12725,592 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>carNight2.wav, 180ms frame,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> w/ null data, with speed optimizations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$A$1:$A$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="105"/>
+                <c:pt idx="0">
+                  <c:v>-5.5143265876445198E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.4337772810048304E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3743975290682198E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8227197273813899E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8142386657762903E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5320393802113996E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.77311912150539E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1685225348688299E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0111392703757995E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.3322397037262699E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1175452032148098E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6331675764272E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.32436352592297E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.7590154966941001E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.1136836644723301E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.77998932842205E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.26966167927675E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8204303778633599E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2225792067933702E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.09556488140052E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4955848471040799E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.7179757234065202E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.30460933197812E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.6246119285491899E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9386615145568502E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0546266722023801E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2177538924448501E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.71587635501422E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.8420061493627702E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2989361763618802E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.5102139843465199E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.4219795394135498E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.2376288735345795E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.2123089034489704E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.8841119455869904E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.7760945200927803E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.7361130749666103E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.1284924269789999E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.4312835243127099E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.112824726154021</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.14389127393516599</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.209127787697408</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.27160204238055002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.33503141024556699</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.42194875679924199</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.53639979769257495</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.62592330204718205</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.72163621914295095</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.68180822995433898</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.93031764929738903</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.82706465041476795</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.92568850532133695</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.86355535961336105</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.97170210089393005</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.04154118137358</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.74214225900972997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.65876526220368203</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.87376897401290499</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.53789809817147105</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.63705401887506</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.1012704337955001E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-4.9272250305436999E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-6.1066837762232097E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-2.65455378701689E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-2.54149683931288E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-3.6864477198306898E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-2.4815960951669502E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-2.5834948287591399E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.158151025904708</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-2.76820172152022E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-2.44543861580005E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-2.0822244233618298E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-1.19488577382202E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-2.0582515929829098E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-2.6915118418017098E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-7.1038380409612304E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-3.3202006310575502E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-2.5180594623108999E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-8.8734016292360801E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-7.3833145226914296E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.200742657090489</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.118462363441589</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-2.8333613301684601E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-1.36695695576157E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-1.06766304882679E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-6.3815098168330704E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-1.24046286052404E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.41224748677984E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.9751544552310301E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-1.85128955692916E-3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.0231248647089901E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-3.3691510851457098E-3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-1.99838851074582E-3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-2.9008879171007599E-3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-8.6460336046241294E-3</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-4.14400383947455E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.14887186166486E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8.9103480268987404E-3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1.24647124476737E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.03175079232123E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-1.33431890384209E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.6116948696752302E-3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-1.88460876424733E-3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>9.7535150245767702E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4.8810653296874297E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="4792560"/>
+        <c:axId val="4793680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="4792560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4793680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="4793680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4792560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12965,6 +13552,46 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -16616,6 +17243,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -16840,6 +17983,41 @@
       <xdr:colOff>276224</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>557211</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32035,7 +33213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A437"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -34230,4 +35408,545 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-5.5143265876445198E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-4.4337772810048304E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.3743975290682198E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.8227197273813899E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8.8142386657762903E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7.5320393802113996E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.77311912150539E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.1685225348688299E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.0111392703757995E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8.3322397037262699E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.1175452032148098E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.6331675764272E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.32436352592297E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9.7590154966941001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5.1136836644723301E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2.77998932842205E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.26966167927675E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2.8204303778633599E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3.2225792067933702E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.09556488140052E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.4955848471040799E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.7179757234065202E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.30460933197812E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2.6246119285491899E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3.9386615145568502E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5.0546266722023801E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2.2177538924448501E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3.71587635501422E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4.8420061493627702E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3.2989361763618802E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7.5102139843465199E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6.4219795394135498E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7.2376288735345795E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>7.2123089034489704E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>6.8841119455869904E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5.7760945200927803E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5.7361130749666103E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>9.1284924269789999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>9.4312835243127099E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.112824726154021</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.14389127393516599</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.209127787697408</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.27160204238055002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.33503141024556699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.42194875679924199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.53639979769257495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.62592330204718205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.72163621914295095</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.68180822995433898</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.93031764929738903</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0.82706465041476795</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0.92568850532133695</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.86355535961336105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.97170210089393005</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1.04154118137358</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.74214225900972997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.65876526220368203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.87376897401290499</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.53789809817147105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1.63705401887506</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1.1012704337955001E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>-4.9272250305436999E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>-6.1066837762232097E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>-2.65455378701689E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>-2.54149683931288E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>-3.6864477198306898E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>-2.4815960951669502E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>-2.5834948287591399E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.158151025904708</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>-2.76820172152022E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>-2.44543861580005E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>-2.0822244233618298E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>-1.19488577382202E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>-2.0582515929829098E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>-2.6915118418017098E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>-7.1038380409612304E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>-3.3202006310575502E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>-2.5180594623108999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>-8.8734016292360801E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>-7.3833145226914296E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>0.200742657090489</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0.118462363441589</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>-2.8333613301684601E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>-1.36695695576157E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>-1.06766304882679E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>-6.3815098168330704E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>-1.24046286052404E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1.41224748677984E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>3.9751544552310301E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>-1.85128955692916E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1.0231248647089901E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>-3.3691510851457098E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>-1.99838851074582E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>-2.9008879171007599E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>-8.6460336046241294E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>-4.14400383947455E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1.14887186166486E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>8.9103480268987404E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>-1.24647124476737E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1.03175079232123E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>-1.33431890384209E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2.6116948696752302E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>-1.88460876424733E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>9.7535150245767702E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>4.8810653296874297E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>